<commit_message>
Update README.md, add .gitignore
</commit_message>
<xml_diff>
--- a/TestCasesForGoogleCom.xlsx
+++ b/TestCasesForGoogleCom.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocuments\Uzduotys isidarbinimui i Junior\QA Tesonet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocuments\Uzduotys isidarbinimui i Junior\TaskSolutionsToJuniorQAinTesonet\TasksSolutionsToJuniorQA\TasksSolutionsToJuniorQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705E4DAF-738E-43D2-A0C7-E0AE7B0176DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEE69BA-3C70-4C5E-A857-79AEE36BFF46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testing environments" sheetId="1" r:id="rId1"/>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t>Chrome Ver. 85.0.4183.83 (Official build) (64-bit)</t>
-  </si>
-  <si>
-    <t>2020.08.31 - 2020.09.04</t>
   </si>
   <si>
     <t>Open page https://www.google.com/</t>
@@ -476,6 +473,9 @@
   </si>
   <si>
     <t>Opens Search Results page (see  "Specific keywords data table")</t>
+  </si>
+  <si>
+    <t>2020.08.31 - 2020.09.01</t>
   </si>
 </sst>
 </file>
@@ -753,25 +753,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -781,8 +763,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -837,18 +817,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -878,6 +848,36 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1735,8 +1735,8 @@
   </sheetPr>
   <dimension ref="A2:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1787,7 +1787,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>69</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1">
@@ -1907,7 +1907,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8:M33"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1969,10 +1969,10 @@
       <c r="AE1" s="9"/>
     </row>
     <row r="2" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="8" t="s">
         <v>21</v>
       </c>
@@ -2008,11 +2008,11 @@
       <c r="AE2" s="9"/>
     </row>
     <row r="3" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="33" t="s">
-        <v>72</v>
+      <c r="D3" s="23" t="s">
+        <v>71</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>23</v>
@@ -2057,11 +2057,11 @@
       <c r="AE3" s="9"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="33" t="s">
-        <v>73</v>
+      <c r="D4" s="23" t="s">
+        <v>72</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>23</v>
@@ -2106,11 +2106,11 @@
       <c r="AE4" s="9"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="34" t="s">
-        <v>74</v>
+      <c r="D5" s="24" t="s">
+        <v>73</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>23</v>
@@ -2155,11 +2155,11 @@
       <c r="AE5" s="9"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="60"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="34" t="s">
-        <v>75</v>
+      <c r="D6" s="24" t="s">
+        <v>74</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>23</v>
@@ -2204,11 +2204,11 @@
       <c r="AE6" s="9"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="60"/>
       <c r="C7" s="11"/>
-      <c r="D7" s="34" t="s">
-        <v>76</v>
+      <c r="D7" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>23</v>
@@ -2253,11 +2253,11 @@
       <c r="AE7" s="9"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
+      <c r="A8" s="59"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="34" t="s">
-        <v>77</v>
+      <c r="D8" s="24" t="s">
+        <v>76</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>23</v>
@@ -2302,13 +2302,13 @@
       <c r="AE8" s="18"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="60"/>
       <c r="C9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="32" t="s">
-        <v>116</v>
+      <c r="D9" s="22" t="s">
+        <v>115</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -2339,11 +2339,11 @@
       <c r="AE9" s="9"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="10"/>
-      <c r="D10" s="33" t="s">
-        <v>103</v>
+      <c r="D10" s="23" t="s">
+        <v>102</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>23</v>
@@ -2388,11 +2388,11 @@
       <c r="AE10" s="9"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
+      <c r="A11" s="59"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="33" t="s">
-        <v>105</v>
+      <c r="D11" s="23" t="s">
+        <v>104</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>23</v>
@@ -2437,11 +2437,11 @@
       <c r="AE11" s="9"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
+      <c r="A12" s="59"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="33" t="s">
-        <v>110</v>
+      <c r="D12" s="23" t="s">
+        <v>109</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>23</v>
@@ -2486,11 +2486,11 @@
       <c r="AE12" s="18"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
+      <c r="A13" s="59"/>
+      <c r="B13" s="60"/>
       <c r="C13" s="13"/>
-      <c r="D13" s="33" t="s">
-        <v>117</v>
+      <c r="D13" s="23" t="s">
+        <v>116</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>23</v>
@@ -2535,13 +2535,13 @@
       <c r="AE13" s="18"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="54" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="22" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="12" t="s">
@@ -2576,11 +2576,11 @@
       <c r="AE14" s="9"/>
     </row>
     <row r="15" spans="1:31" ht="12.75">
-      <c r="A15" s="22"/>
+      <c r="A15" s="55"/>
       <c r="B15" s="8"/>
       <c r="C15" s="10"/>
-      <c r="D15" s="34" t="s">
-        <v>124</v>
+      <c r="D15" s="24" t="s">
+        <v>123</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -2615,21 +2615,21 @@
       <c r="AE15" s="9"/>
     </row>
     <row r="16" spans="1:31" ht="12.75">
-      <c r="A16" s="22"/>
+      <c r="A16" s="55"/>
       <c r="B16" s="8"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="34" t="s">
-        <v>125</v>
+      <c r="D16" s="24" t="s">
+        <v>124</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="33" t="s">
+      <c r="J16" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="33" t="s">
+      <c r="K16" s="23" t="s">
         <v>25</v>
       </c>
       <c r="L16" s="9"/>
@@ -2654,9 +2654,9 @@
       <c r="AE16" s="9"/>
     </row>
     <row r="17" spans="1:31" ht="12.75">
-      <c r="A17" s="22"/>
+      <c r="A17" s="55"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="22" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="12" t="s">
@@ -2691,13 +2691,13 @@
       <c r="AE17" s="9"/>
     </row>
     <row r="18" spans="1:31" ht="25.5">
-      <c r="A18" s="22"/>
+      <c r="A18" s="55"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="34" t="s">
-        <v>130</v>
+      <c r="D18" s="24" t="s">
+        <v>129</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="23" t="s">
         <v>23</v>
       </c>
       <c r="F18" s="10" t="s">
@@ -2740,11 +2740,11 @@
       <c r="AE18" s="9"/>
     </row>
     <row r="19" spans="1:31" ht="12.75">
-      <c r="A19" s="22"/>
+      <c r="A19" s="55"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
-      <c r="D19" s="34" t="s">
-        <v>131</v>
+      <c r="D19" s="24" t="s">
+        <v>130</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>23</v>
@@ -2785,13 +2785,13 @@
       <c r="AE19" s="18"/>
     </row>
     <row r="20" spans="1:31" ht="25.5">
-      <c r="A20" s="22"/>
+      <c r="A20" s="55"/>
       <c r="B20" s="8"/>
       <c r="C20" s="10"/>
-      <c r="D20" s="34" t="s">
-        <v>132</v>
+      <c r="D20" s="24" t="s">
+        <v>131</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="23" t="s">
         <v>25</v>
       </c>
       <c r="F20" s="10" t="s">
@@ -2800,7 +2800,7 @@
       <c r="G20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="23" t="s">
         <v>25</v>
       </c>
       <c r="I20" s="10" t="s">
@@ -2830,11 +2830,11 @@
       <c r="AE20" s="9"/>
     </row>
     <row r="21" spans="1:31" ht="12.75">
-      <c r="A21" s="22"/>
+      <c r="A21" s="55"/>
       <c r="B21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="22" t="s">
         <v>28</v>
       </c>
       <c r="D21" s="12" t="s">
@@ -2869,11 +2869,11 @@
       <c r="AE21" s="9"/>
     </row>
     <row r="22" spans="1:31" ht="12.75">
-      <c r="A22" s="22"/>
+      <c r="A22" s="55"/>
       <c r="B22" s="13"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="34" t="s">
-        <v>138</v>
+      <c r="D22" s="24" t="s">
+        <v>137</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>23</v>
@@ -2918,11 +2918,11 @@
       <c r="AE22" s="9"/>
     </row>
     <row r="23" spans="1:31" ht="12.75">
-      <c r="A23" s="22"/>
+      <c r="A23" s="55"/>
       <c r="B23" s="13"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="34" t="s">
-        <v>139</v>
+      <c r="D23" s="24" t="s">
+        <v>138</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>23</v>
@@ -2967,11 +2967,11 @@
       <c r="AE23" s="9"/>
     </row>
     <row r="24" spans="1:31" ht="12.75">
-      <c r="A24" s="22"/>
+      <c r="A24" s="55"/>
       <c r="B24" s="13"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="33" t="s">
-        <v>140</v>
+      <c r="D24" s="23" t="s">
+        <v>139</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>23</v>
@@ -3016,9 +3016,9 @@
       <c r="AE24" s="9"/>
     </row>
     <row r="25" spans="1:31" ht="12.75">
-      <c r="A25" s="22"/>
+      <c r="A25" s="55"/>
       <c r="B25" s="13"/>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="22" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="8" t="s">
@@ -3053,11 +3053,11 @@
       <c r="AE25" s="9"/>
     </row>
     <row r="26" spans="1:31" ht="12.75">
-      <c r="A26" s="23"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="13"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="33" t="s">
-        <v>141</v>
+      <c r="D26" s="23" t="s">
+        <v>140</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>23</v>
@@ -3105,8 +3105,8 @@
       <c r="A27" s="14"/>
       <c r="B27" s="13"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="34" t="s">
-        <v>142</v>
+      <c r="D27" s="24" t="s">
+        <v>141</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>25</v>
@@ -3153,7 +3153,7 @@
     <row r="28" spans="1:31" ht="12.75">
       <c r="A28" s="14"/>
       <c r="B28" s="13"/>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="22" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="8" t="s">
@@ -3191,8 +3191,8 @@
       <c r="A29" s="14"/>
       <c r="B29" s="13"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="34" t="s">
-        <v>143</v>
+      <c r="D29" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>23</v>
@@ -3240,8 +3240,8 @@
       <c r="A30" s="14"/>
       <c r="B30" s="13"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="33" t="s">
-        <v>144</v>
+      <c r="D30" s="23" t="s">
+        <v>143</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>23</v>
@@ -3289,8 +3289,8 @@
       <c r="A31" s="14"/>
       <c r="B31" s="13"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="33" t="s">
-        <v>145</v>
+      <c r="D31" s="23" t="s">
+        <v>144</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>23</v>
@@ -3337,7 +3337,7 @@
     <row r="32" spans="1:31" ht="12.75">
       <c r="A32" s="14"/>
       <c r="B32" s="13"/>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="22" t="s">
         <v>34</v>
       </c>
       <c r="D32" s="8" t="s">
@@ -3375,8 +3375,8 @@
       <c r="A33" s="14"/>
       <c r="B33" s="13"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="34" t="s">
-        <v>146</v>
+      <c r="D33" s="24" t="s">
+        <v>145</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>23</v>
@@ -3497,8 +3497,8 @@
       <c r="B36" s="17">
         <v>1</v>
       </c>
-      <c r="C36" s="47" t="s">
-        <v>147</v>
+      <c r="C36" s="35" t="s">
+        <v>146</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="9"/>
@@ -34617,8 +34617,8 @@
   </sheetPr>
   <dimension ref="A1:AG994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
@@ -34635,10 +34635,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="65"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -34672,10 +34672,10 @@
       <c r="AG1" s="9"/>
     </row>
     <row r="2" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A2" s="31" t="s">
-        <v>71</v>
+      <c r="A2" s="66" t="s">
+        <v>70</v>
       </c>
-      <c r="B2" s="29"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
@@ -34709,10 +34709,10 @@
       <c r="AG2" s="18"/>
     </row>
     <row r="3" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A3" s="31" t="s">
-        <v>70</v>
+      <c r="A3" s="66" t="s">
+        <v>69</v>
       </c>
-      <c r="B3" s="29"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -34781,10 +34781,10 @@
       <c r="AG4" s="9"/>
     </row>
     <row r="5" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="29"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -34818,10 +34818,10 @@
       <c r="AG5" s="9"/>
     </row>
     <row r="6" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A6" s="31" t="s">
-        <v>71</v>
+      <c r="A6" s="66" t="s">
+        <v>70</v>
       </c>
-      <c r="B6" s="29"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
@@ -34855,10 +34855,10 @@
       <c r="AG6" s="18"/>
     </row>
     <row r="7" spans="1:33" ht="15.75" customHeight="1">
-      <c r="A7" s="31" t="s">
-        <v>70</v>
+      <c r="A7" s="66" t="s">
+        <v>69</v>
       </c>
-      <c r="B7" s="29"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -34927,46 +34927,46 @@
       <c r="AG8" s="9"/>
     </row>
     <row r="9" spans="1:33" ht="25.5">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="E9" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="49" t="s">
+      <c r="H9" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="49" t="s">
+      <c r="I9" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="49" t="s">
+      <c r="J9" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="49" t="s">
+      <c r="K9" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="L9" s="49" t="s">
+      <c r="L9" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="M9" s="49" t="s">
+      <c r="M9" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="N9" s="48" t="s">
+      <c r="N9" s="36" t="s">
         <v>59</v>
       </c>
       <c r="O9" s="9"/>
@@ -34990,44 +34990,44 @@
       <c r="AG9" s="9"/>
     </row>
     <row r="10" spans="1:33" ht="63.75">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="C10" s="40">
+        <v>1</v>
+      </c>
+      <c r="D10" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="52">
-        <v>1</v>
-      </c>
-      <c r="D10" s="53" t="s">
+      <c r="E10" s="42"/>
+      <c r="F10" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="53" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="52" t="s">
+      <c r="G10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="52" t="s">
+      <c r="H10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="52" t="s">
+      <c r="I10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="52" t="s">
+      <c r="J10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="52" t="s">
+      <c r="K10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="52" t="s">
+      <c r="L10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="M10" s="52" t="s">
+      <c r="M10" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="52"/>
+      <c r="N10" s="40"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
@@ -35049,30 +35049,30 @@
       <c r="AG10" s="9"/>
     </row>
     <row r="11" spans="1:33" ht="25.5">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="56" t="s">
-        <v>101</v>
+      <c r="B11" s="63" t="s">
+        <v>100</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="40">
         <v>1</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
@@ -35094,40 +35094,40 @@
       <c r="AG11" s="9"/>
     </row>
     <row r="12" spans="1:33" ht="38.25">
-      <c r="A12" s="58"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="52">
+      <c r="A12" s="62"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="40">
         <v>2</v>
       </c>
-      <c r="D12" s="53" t="s">
-        <v>102</v>
+      <c r="D12" s="41" t="s">
+        <v>101</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53" t="s">
-        <v>148</v>
+      <c r="E12" s="40"/>
+      <c r="F12" s="41" t="s">
+        <v>147</v>
       </c>
-      <c r="G12" s="52" t="s">
+      <c r="G12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="52" t="s">
+      <c r="H12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="52" t="s">
+      <c r="I12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="52" t="s">
+      <c r="J12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="52" t="s">
+      <c r="K12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="52" t="s">
+      <c r="L12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="52" t="s">
+      <c r="M12" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="52"/>
+      <c r="N12" s="40"/>
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
@@ -35149,30 +35149,30 @@
       <c r="AG12" s="9"/>
     </row>
     <row r="13" spans="1:33" ht="25.5">
-      <c r="A13" s="59" t="s">
-        <v>104</v>
+      <c r="A13" s="61" t="s">
+        <v>103</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="40">
+        <v>1</v>
+      </c>
+      <c r="D13" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="C13" s="52">
-        <v>1</v>
-      </c>
-      <c r="D13" s="53" t="s">
+      <c r="E13" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="E13" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
       <c r="O13" s="18"/>
       <c r="P13" s="18"/>
       <c r="Q13" s="18"/>
@@ -35194,40 +35194,40 @@
       <c r="AG13" s="18"/>
     </row>
     <row r="14" spans="1:33" ht="51">
-      <c r="A14" s="58"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="52">
+      <c r="A14" s="62"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="40">
         <v>2</v>
       </c>
-      <c r="D14" s="53" t="s">
-        <v>102</v>
+      <c r="D14" s="41" t="s">
+        <v>101</v>
       </c>
-      <c r="E14" s="52"/>
-      <c r="F14" s="53" t="s">
-        <v>109</v>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41" t="s">
+        <v>108</v>
       </c>
-      <c r="G14" s="52" t="s">
+      <c r="G14" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="52" t="s">
+      <c r="H14" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="52" t="s">
+      <c r="I14" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="52" t="s">
+      <c r="J14" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="52" t="s">
+      <c r="K14" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="L14" s="52" t="s">
+      <c r="L14" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="M14" s="52" t="s">
+      <c r="M14" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N14" s="52"/>
+      <c r="N14" s="40"/>
       <c r="O14" s="18"/>
       <c r="P14" s="18"/>
       <c r="Q14" s="18"/>
@@ -35249,30 +35249,30 @@
       <c r="AG14" s="18"/>
     </row>
     <row r="15" spans="1:33" ht="25.5">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="C15" s="40">
+        <v>1</v>
+      </c>
+      <c r="D15" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="52">
-        <v>1</v>
-      </c>
-      <c r="D15" s="53" t="s">
+      <c r="E15" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="E15" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" s="51"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
       <c r="O15" s="18"/>
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
@@ -35294,40 +35294,40 @@
       <c r="AG15" s="18"/>
     </row>
     <row r="16" spans="1:33" ht="38.25">
-      <c r="A16" s="58"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="52">
+      <c r="A16" s="62"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="40">
         <v>2</v>
       </c>
-      <c r="D16" s="53" t="s">
-        <v>102</v>
+      <c r="D16" s="41" t="s">
+        <v>101</v>
       </c>
-      <c r="E16" s="52"/>
-      <c r="F16" s="53" t="s">
-        <v>115</v>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41" t="s">
+        <v>114</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="52" t="s">
+      <c r="H16" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="52" t="s">
+      <c r="I16" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="J16" s="52" t="s">
+      <c r="J16" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="52" t="s">
+      <c r="K16" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="L16" s="52" t="s">
+      <c r="L16" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="M16" s="52" t="s">
+      <c r="M16" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="52"/>
+      <c r="N16" s="40"/>
       <c r="O16" s="18"/>
       <c r="P16" s="18"/>
       <c r="Q16" s="18"/>
@@ -35349,30 +35349,30 @@
       <c r="AG16" s="18"/>
     </row>
     <row r="17" spans="1:33" ht="25.5">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="B17" s="56" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="52">
+      <c r="C17" s="40">
         <v>1</v>
       </c>
-      <c r="D17" s="62" t="s">
+      <c r="D17" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="E17" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="52"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
       <c r="Q17" s="9"/>
@@ -35394,40 +35394,40 @@
       <c r="AG17" s="9"/>
     </row>
     <row r="18" spans="1:33" ht="25.5">
-      <c r="A18" s="58"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="52">
+      <c r="A18" s="62"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="40">
         <v>2</v>
       </c>
-      <c r="D18" s="53" t="s">
-        <v>102</v>
+      <c r="D18" s="41" t="s">
+        <v>101</v>
       </c>
-      <c r="E18" s="52"/>
-      <c r="F18" s="53" t="s">
-        <v>100</v>
+      <c r="E18" s="40"/>
+      <c r="F18" s="41" t="s">
+        <v>99</v>
       </c>
-      <c r="G18" s="52" t="s">
+      <c r="G18" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="52" t="s">
+      <c r="H18" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="52" t="s">
+      <c r="I18" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="52" t="s">
+      <c r="J18" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="52" t="s">
+      <c r="K18" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="52" t="s">
+      <c r="L18" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="M18" s="52" t="s">
+      <c r="M18" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N18" s="52"/>
+      <c r="N18" s="40"/>
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
@@ -35449,36 +35449,36 @@
       <c r="AG18" s="9"/>
     </row>
     <row r="19" spans="1:33" ht="25.5">
-      <c r="A19" s="58"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="52">
+      <c r="A19" s="62"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="40">
         <v>3.1</v>
       </c>
-      <c r="D19" s="51" t="s">
-        <v>122</v>
+      <c r="D19" s="39" t="s">
+        <v>121</v>
       </c>
-      <c r="E19" s="52"/>
-      <c r="F19" s="53" t="s">
-        <v>120</v>
+      <c r="E19" s="40"/>
+      <c r="F19" s="41" t="s">
+        <v>119</v>
       </c>
-      <c r="G19" s="52" t="s">
+      <c r="G19" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="52" t="s">
+      <c r="H19" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="52" t="s">
+      <c r="I19" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="52" t="s">
+      <c r="J19" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="52" t="s">
+      <c r="K19" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="52"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
       <c r="O19" s="18"/>
       <c r="P19" s="18"/>
       <c r="Q19" s="18"/>
@@ -35500,30 +35500,30 @@
       <c r="AG19" s="18"/>
     </row>
     <row r="20" spans="1:33" ht="25.5">
-      <c r="A20" s="58"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="52">
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="40">
         <v>3.2</v>
       </c>
-      <c r="D20" s="51" t="s">
-        <v>121</v>
+      <c r="D20" s="39" t="s">
+        <v>120</v>
       </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="53" t="s">
-        <v>123</v>
+      <c r="E20" s="40"/>
+      <c r="F20" s="41" t="s">
+        <v>122</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52" t="s">
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="M20" s="52" t="s">
+      <c r="M20" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="N20" s="52"/>
+      <c r="N20" s="40"/>
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
@@ -35545,35 +35545,35 @@
       <c r="AG20" s="9"/>
     </row>
     <row r="21" spans="1:33" ht="25.5">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="40">
+        <v>1</v>
+      </c>
+      <c r="D21" s="41" t="s">
         <v>126</v>
       </c>
-      <c r="C21" s="52">
-        <v>1</v>
-      </c>
-      <c r="D21" s="53" t="s">
+      <c r="E21" s="42"/>
+      <c r="F21" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="E21" s="54"/>
-      <c r="F21" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="51" t="s">
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="M21" s="51" t="s">
+      <c r="M21" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="N21" s="53" t="s">
-        <v>129</v>
+      <c r="N21" s="41" t="s">
+        <v>128</v>
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
@@ -35596,41 +35596,41 @@
       <c r="AG21" s="9"/>
     </row>
     <row r="22" spans="1:33" ht="38.25">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="C22" s="40">
+        <v>1</v>
+      </c>
+      <c r="D22" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="C22" s="52">
-        <v>1</v>
-      </c>
-      <c r="D22" s="53" t="s">
+      <c r="E22" s="47"/>
+      <c r="F22" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="53" t="s">
-        <v>136</v>
-      </c>
-      <c r="G22" s="51" t="s">
+      <c r="G22" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="52" t="s">
+      <c r="H22" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="52" t="s">
+      <c r="I22" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="J22" s="51" t="s">
+      <c r="J22" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="52" t="s">
+      <c r="K22" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="53" t="s">
-        <v>137</v>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="41" t="s">
+        <v>136</v>
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
@@ -36422,7 +36422,7 @@
       <c r="AF44" s="9"/>
       <c r="AG44" s="9"/>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:33" ht="12.75">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -69680,20 +69680,20 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="14">
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B17:B20"/>
   </mergeCells>
   <conditionalFormatting sqref="G10:M12 G17:M25">
     <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="Pass">
@@ -69747,205 +69747,205 @@
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" style="46" customWidth="1"/>
-    <col min="4" max="10" width="8" style="68" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="34" customWidth="1"/>
+    <col min="4" max="10" width="8" style="52" customWidth="1"/>
     <col min="11" max="11" width="51.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="21"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="21"/>
+    </row>
+    <row r="3" spans="1:11" ht="25.5">
+      <c r="A3" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="25.5">
+      <c r="A4" s="53" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="30"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="30"/>
-    </row>
-    <row r="3" spans="1:11" ht="25.5">
-      <c r="A3" s="37" t="s">
-        <v>82</v>
+      <c r="C4" s="33" t="s">
+        <v>90</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>83</v>
+      <c r="D4" s="50" t="s">
+        <v>23</v>
       </c>
-      <c r="C3" s="37" t="s">
-        <v>84</v>
+      <c r="E4" s="50" t="s">
+        <v>23</v>
       </c>
-      <c r="D3" s="64" t="s">
-        <v>52</v>
+      <c r="F4" s="50" t="s">
+        <v>23</v>
       </c>
-      <c r="E3" s="64" t="s">
-        <v>53</v>
+      <c r="G4" s="50" t="s">
+        <v>23</v>
       </c>
-      <c r="F3" s="64" t="s">
-        <v>54</v>
+      <c r="H4" s="50" t="s">
+        <v>23</v>
       </c>
-      <c r="G3" s="64" t="s">
-        <v>55</v>
+      <c r="I4" s="50" t="s">
+        <v>23</v>
       </c>
-      <c r="H3" s="64" t="s">
-        <v>56</v>
+      <c r="J4" s="50" t="s">
+        <v>23</v>
       </c>
-      <c r="I3" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="38" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="25.5">
-      <c r="A4" s="69" t="s">
+      <c r="K4" s="28"/>
+    </row>
+    <row r="5" spans="1:11" ht="25.5">
+      <c r="A5" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="45" t="s">
+      <c r="B5" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="C5" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="E5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="66" t="s">
+      <c r="F5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="66" t="s">
+      <c r="G5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="66" t="s">
+      <c r="H5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="66" t="s">
+      <c r="I5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="66" t="s">
+      <c r="J5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="40"/>
-    </row>
-    <row r="5" spans="1:11" ht="25.5">
-      <c r="A5" s="69" t="s">
+      <c r="K5" s="28"/>
+    </row>
+    <row r="6" spans="1:11" ht="25.5">
+      <c r="A6" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="42" t="s">
+      <c r="B6" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="67" t="s">
+      <c r="C6" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="67" t="s">
+      <c r="E6" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="67" t="s">
+      <c r="F6" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G6" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="67" t="s">
+      <c r="H6" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I6" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="67" t="s">
+      <c r="J6" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="40"/>
-    </row>
-    <row r="6" spans="1:11" ht="25.5">
-      <c r="A6" s="69" t="s">
+      <c r="K6" s="28"/>
+    </row>
+    <row r="7" spans="1:11" ht="38.25">
+      <c r="A7" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B7" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="42" t="s">
-        <v>97</v>
+      <c r="C7" s="30" t="s">
+        <v>95</v>
       </c>
-      <c r="D6" s="67" t="s">
+      <c r="D7" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="67" t="s">
+      <c r="E7" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="67" t="s">
+      <c r="F7" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="67" t="s">
+      <c r="G7" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="67" t="s">
+      <c r="H7" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="67" t="s">
+      <c r="I7" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="67" t="s">
+      <c r="J7" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="40"/>
-    </row>
-    <row r="7" spans="1:11" ht="38.25">
-      <c r="A7" s="69" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="40"/>
+      <c r="K7" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>